<commit_message>
excel basicamente terminado, exceto erro do excel
</commit_message>
<xml_diff>
--- a/pONG-painel_de_controle/src/php_stuff/hello world.xlsx
+++ b/pONG-painel_de_controle/src/php_stuff/hello world.xlsx
@@ -15,9 +15,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
-  <si>
-    <t>Hello World !</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+  <si>
+    <t>Gatinhos para doação - 2022-07-29 21:43:42</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>E-Mail</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>Data De Nascimento</t>
+  </si>
+  <si>
+    <t>Profissão</t>
+  </si>
+  <si>
+    <t>Sexo</t>
+  </si>
+  <si>
+    <t>Cidade</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Pedro Henrique M. Virtuozo</t>
+  </si>
+  <si>
+    <t>pedrovirtuozo@gmail.com</t>
+  </si>
+  <si>
+    <t>2004-05-19</t>
+  </si>
+  <si>
+    <t>Estudante</t>
+  </si>
+  <si>
+    <t>OUTR</t>
+  </si>
+  <si>
+    <t>Criciúma</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>cadu</t>
+  </si>
+  <si>
+    <t>cadedu@gmail.com</t>
+  </si>
+  <si>
+    <t>2022-02-01</t>
+  </si>
+  <si>
+    <t>MASC</t>
   </si>
 </sst>
 </file>
@@ -25,23 +82,50 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor rgb="FFC6E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EA9DB"/>
+        <bgColor rgb="FF8EA9DB"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -50,9 +134,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -353,21 +449,120 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B6" sqref="B6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="2" max="2" width="2" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="30" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="27" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="21" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="5" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="7" bestFit="true" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="3" spans="1:10">
+      <c r="B3" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5548996234350</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4">
+        <v>356457467</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="B3:J3"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
início de gerar pdf
</commit_message>
<xml_diff>
--- a/pONG-painel_de_controle/src/php_stuff/hello world.xlsx
+++ b/pONG-painel_de_controle/src/php_stuff/hello world.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
-  <si>
-    <t>Gatinhos para doação - 2022-07-29 21:43:42</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+  <si>
+    <t>Teste de Evento 2 - 2022-09-26 10:15:15</t>
   </si>
   <si>
     <t>Nome</t>
@@ -63,18 +63,6 @@
   </si>
   <si>
     <t>SC</t>
-  </si>
-  <si>
-    <t>cadu</t>
-  </si>
-  <si>
-    <t>cadedu@gmail.com</t>
-  </si>
-  <si>
-    <t>2022-02-01</t>
-  </si>
-  <si>
-    <t>MASC</t>
   </si>
 </sst>
 </file>
@@ -102,7 +90,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,12 +109,6 @@
         <bgColor rgb="FFD9E1F2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8EA9DB"/>
-        <bgColor rgb="FF8EA9DB"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -134,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -145,9 +127,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -449,10 +428,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B6" sqref="B6:J6"/>
+      <selection activeCell="B5" sqref="B5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -526,35 +505,6 @@
         <v>14</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="B6" s="4">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="4">
-        <v>356457467</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="4" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionando a parte de comentarios no painel de controle
</commit_message>
<xml_diff>
--- a/pONG-painel_de_controle/src/php_stuff/hello world.xlsx
+++ b/pONG-painel_de_controle/src/php_stuff/hello world.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Campanha do Agasalho 2022 - 2022-10-27 11:27:21</t>
   </si>
@@ -44,43 +44,28 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>Pedro Henrique Sand Cardoso</t>
-  </si>
-  <si>
-    <t>pedrovirtuozo@gmail.com</t>
-  </si>
-  <si>
-    <t>+55 (48) 99623-4350</t>
-  </si>
-  <si>
-    <t>2004-05-19</t>
+    <t>Carlinhos</t>
+  </si>
+  <si>
+    <t>carlinhos@gmail.com</t>
+  </si>
+  <si>
+    <t>(48) 99999-9999</t>
+  </si>
+  <si>
+    <t>2005-11-15</t>
   </si>
   <si>
     <t>Estudante</t>
   </si>
   <si>
-    <t>OUTR</t>
-  </si>
-  <si>
-    <t>Criciúma</t>
+    <t>MASC</t>
+  </si>
+  <si>
+    <t>Criciuma</t>
   </si>
   <si>
     <t>SC</t>
-  </si>
-  <si>
-    <t>Carlos Edudardo</t>
-  </si>
-  <si>
-    <t>carlos@gmail.com</t>
-  </si>
-  <si>
-    <t>2006-03-30</t>
-  </si>
-  <si>
-    <t>MASC</t>
-  </si>
-  <si>
-    <t>Criciuma</t>
   </si>
 </sst>
 </file>
@@ -108,7 +93,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,12 +112,6 @@
         <bgColor rgb="FFD9E1F2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8EA9DB"/>
-        <bgColor rgb="FF8EA9DB"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -140,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -151,9 +130,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -455,18 +431,18 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B6" sqref="B6:J6"/>
+      <selection activeCell="B5" sqref="B5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="2" max="2" width="2" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="31" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="27" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="22" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="22" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="18" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="21" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="11" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="5" bestFit="true" customWidth="true" style="0"/>
@@ -532,35 +508,6 @@
         <v>15</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="B6" s="4">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="4">
-        <v>12345</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="4" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>